<commit_message>
Ajustes losas modelo y avance en dimension losas
</commit_message>
<xml_diff>
--- a/Tarea 05/dimensiones losas.xlsx
+++ b/Tarea 05/dimensiones losas.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive (ignacio.yanez.g@ug.uchile.cl)\Universidad\Semestre 12 Primavera 2018\proyecto de hormigon\proyecto-CI5206\Tarea 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CCA496-B794-4058-B93B-C51D206845CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B0117A-F854-41D0-8174-1DD83B10C322}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{77A8B211-3B65-4AFE-BDB5-07A2739F3869}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="2" xr2:uid="{77A8B211-3B65-4AFE-BDB5-07A2739F3869}"/>
   </bookViews>
   <sheets>
     <sheet name="Piso -1" sheetId="1" r:id="rId1"/>
     <sheet name="Piso 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Piso 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
   <si>
     <t>N° Losa</t>
   </si>
@@ -208,6 +209,78 @@
   </si>
   <si>
     <t>120</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>218</t>
+  </si>
+  <si>
+    <t>219</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>222</t>
   </si>
 </sst>
 </file>
@@ -249,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,6 +331,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7796671-BE69-4D9A-8979-89DC1EB38DCD}">
   <dimension ref="B3:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H32"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1334,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB8B69-A653-4E8B-A8D1-A28FAE860C51}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E29:E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,10 +1450,10 @@
         <v>5.33</v>
       </c>
       <c r="E3" s="1">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="G3" s="1">
         <v>500</v>
@@ -1397,7 +1473,7 @@
         <v>7.2</v>
       </c>
       <c r="E4" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1">
         <v>6</v>
@@ -1420,7 +1496,7 @@
         <v>7.2</v>
       </c>
       <c r="E5" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
         <v>6</v>
@@ -1443,7 +1519,7 @@
         <v>7.89</v>
       </c>
       <c r="E6" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1">
         <v>6</v>
@@ -1460,16 +1536,16 @@
         <v>43</v>
       </c>
       <c r="C7" s="1">
-        <v>4.45</v>
+        <v>4.93</v>
       </c>
       <c r="D7" s="1">
-        <v>5</v>
+        <v>5.33</v>
       </c>
       <c r="E7" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
         <v>500</v>
@@ -1483,13 +1559,13 @@
         <v>44</v>
       </c>
       <c r="C8" s="1">
-        <v>3.6</v>
+        <v>5.54</v>
       </c>
       <c r="D8" s="1">
-        <v>5</v>
+        <v>7.2</v>
       </c>
       <c r="E8" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1">
         <v>6</v>
@@ -1506,13 +1582,13 @@
         <v>45</v>
       </c>
       <c r="C9" s="1">
-        <v>5.33</v>
+        <v>5.54</v>
       </c>
       <c r="D9" s="1">
-        <v>5.54</v>
+        <v>7.2</v>
       </c>
       <c r="E9" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1">
         <v>6</v>
@@ -1532,10 +1608,10 @@
         <v>5.54</v>
       </c>
       <c r="D10" s="1">
-        <v>7.2</v>
+        <v>7.89</v>
       </c>
       <c r="E10" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1">
         <v>6</v>
@@ -1555,13 +1631,13 @@
         <v>5.54</v>
       </c>
       <c r="D11" s="1">
-        <v>7.2</v>
+        <v>4.45</v>
       </c>
       <c r="E11" s="1">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G11" s="1">
         <v>500</v>
@@ -1575,19 +1651,19 @@
         <v>48</v>
       </c>
       <c r="C12" s="1">
-        <v>5.54</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="D12" s="1">
-        <v>12.34</v>
+        <v>5.6</v>
       </c>
       <c r="E12" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="1">
         <v>6</v>
       </c>
       <c r="G12" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -1598,13 +1674,13 @@
         <v>49</v>
       </c>
       <c r="C13" s="1">
-        <v>3.6</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="D13" s="1">
-        <v>5.54</v>
+        <v>5.6</v>
       </c>
       <c r="E13" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="1">
         <v>6</v>
@@ -1624,16 +1700,16 @@
         <v>6.05</v>
       </c>
       <c r="D14" s="1">
-        <v>9.34</v>
+        <v>9.49</v>
       </c>
       <c r="E14" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="1">
         <v>6</v>
       </c>
       <c r="G14" s="1">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>32</v>
@@ -1644,16 +1720,16 @@
         <v>51</v>
       </c>
       <c r="C15" s="1">
-        <v>4.6500000000000004</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>5.6</v>
+        <v>2.8250000000000002</v>
       </c>
       <c r="E15" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G15" s="1">
         <v>400</v>
@@ -1667,19 +1743,19 @@
         <v>52</v>
       </c>
       <c r="C16" s="1">
-        <v>4.6500000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="D16" s="1">
-        <v>5.6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E16" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="1">
         <v>6</v>
       </c>
       <c r="G16" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>32</v>
@@ -1690,19 +1766,19 @@
         <v>53</v>
       </c>
       <c r="C17" s="1">
-        <v>6.05</v>
+        <v>2.9</v>
       </c>
       <c r="D17" s="1">
-        <v>9.49</v>
+        <v>6.36</v>
       </c>
       <c r="E17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="1">
         <v>6</v>
       </c>
       <c r="G17" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -1713,19 +1789,19 @@
         <v>54</v>
       </c>
       <c r="C18" s="1">
-        <v>4.45</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1">
-        <v>10.5</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="E18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="1">
         <v>6</v>
       </c>
       <c r="G18" s="1">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>32</v>
@@ -1736,19 +1812,19 @@
         <v>55</v>
       </c>
       <c r="C19" s="1">
-        <v>3.6</v>
+        <v>5.82</v>
       </c>
       <c r="D19" s="1">
-        <v>10.5</v>
+        <v>6.49</v>
       </c>
       <c r="E19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="1">
         <v>6</v>
       </c>
       <c r="G19" s="1">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -1759,19 +1835,19 @@
         <v>56</v>
       </c>
       <c r="C20" s="1">
-        <v>7.16</v>
+        <v>1.34</v>
       </c>
       <c r="D20" s="1">
-        <v>11.34</v>
+        <v>7.01</v>
       </c>
       <c r="E20" s="1">
-        <v>17</v>
-      </c>
-      <c r="F20" s="1">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G20" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>32</v>
@@ -1782,16 +1858,16 @@
         <v>57</v>
       </c>
       <c r="C21" s="1">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="D21" s="1">
-        <v>11.2</v>
+        <v>4.04</v>
       </c>
       <c r="E21" s="1">
-        <v>17</v>
-      </c>
-      <c r="F21" s="1">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G21" s="1">
         <v>400</v>
@@ -1805,16 +1881,16 @@
         <v>58</v>
       </c>
       <c r="C22" s="1">
-        <v>2.1</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="D22" s="1">
-        <v>4.04</v>
+        <v>4.3</v>
       </c>
       <c r="E22" s="1">
-        <v>17</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+      <c r="F22" s="4">
+        <v>6</v>
       </c>
       <c r="G22" s="1">
         <v>400</v>
@@ -1907,4 +1983,548 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CFD12D-4AE1-4F93-8131-51CD10C27189}">
+  <dimension ref="B2:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1">
+        <v>200</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>200</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>200</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>200</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.96</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
+        <v>200</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.04</v>
+      </c>
+      <c r="E9" s="1">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1">
+        <v>400</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>500</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6.36</v>
+      </c>
+      <c r="E11" s="1">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1">
+        <v>500</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>400</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>500</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.33</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6</v>
+      </c>
+      <c r="G14" s="1">
+        <v>500</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1">
+        <v>400</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1">
+        <v>400</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1">
+        <v>400</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1">
+        <v>200</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1">
+        <v>200</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7.01</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1">
+        <v>300</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7.09</v>
+      </c>
+      <c r="E21" s="1">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="1">
+        <v>400</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1">
+        <v>400</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E23" s="1">
+        <v>16</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="1">
+        <v>400</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1">
+        <v>400</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DImensiones de losas y condiciones de apoyo terminadas hasta piso 2
</commit_message>
<xml_diff>
--- a/Tarea 05/dimensiones losas.xlsx
+++ b/Tarea 05/dimensiones losas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive (ignacio.yanez.g@ug.uchile.cl)\Universidad\Semestre 12 Primavera 2018\proyecto de hormigon\proyecto-CI5206\Tarea 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B0117A-F854-41D0-8174-1DD83B10C322}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57F8817-36FD-4BBA-9214-8A3CB3181D59}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="2" xr2:uid="{77A8B211-3B65-4AFE-BDB5-07A2739F3869}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{77A8B211-3B65-4AFE-BDB5-07A2739F3869}"/>
   </bookViews>
   <sheets>
     <sheet name="Piso -1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
   <si>
     <t>N° Losa</t>
   </si>
@@ -701,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7796671-BE69-4D9A-8979-89DC1EB38DCD}">
   <dimension ref="B3:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1411,7 +1411,7 @@
   <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CFD12D-4AE1-4F93-8131-51CD10C27189}">
   <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2196,7 +2196,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>32</v>
@@ -2215,11 +2215,11 @@
       <c r="E11" s="1">
         <v>16</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>38</v>
+      <c r="F11" s="1">
+        <v>6</v>
       </c>
       <c r="G11" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -2242,7 +2242,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -2265,7 +2265,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="1">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>32</v>
@@ -2284,11 +2284,11 @@
       <c r="E14" s="1">
         <v>16</v>
       </c>
-      <c r="F14" s="1">
-        <v>6</v>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G14" s="1">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>32</v>
@@ -2307,11 +2307,11 @@
       <c r="E15" s="1">
         <v>16</v>
       </c>
-      <c r="F15" s="1">
-        <v>4</v>
+      <c r="F15" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G15" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>32</v>
@@ -2330,11 +2330,11 @@
       <c r="E16" s="1">
         <v>16</v>
       </c>
-      <c r="F16" s="1">
-        <v>6</v>
+      <c r="F16" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G16" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>32</v>
@@ -2353,11 +2353,11 @@
       <c r="E17" s="1">
         <v>16</v>
       </c>
-      <c r="F17" s="1">
-        <v>6</v>
+      <c r="F17" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G17" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -2376,11 +2376,11 @@
       <c r="E18" s="1">
         <v>16</v>
       </c>
-      <c r="F18" s="1">
-        <v>6</v>
+      <c r="F18" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G18" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>32</v>
@@ -2399,11 +2399,11 @@
       <c r="E19" s="1">
         <v>16</v>
       </c>
-      <c r="F19" s="1">
-        <v>6</v>
+      <c r="F19" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G19" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>32</v>
@@ -2446,10 +2446,10 @@
         <v>16</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="G21" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>32</v>
@@ -2468,11 +2468,11 @@
       <c r="E22" s="1">
         <v>16</v>
       </c>
-      <c r="F22" s="4">
-        <v>6</v>
+      <c r="F22" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="G22" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>32</v>
@@ -2492,10 +2492,10 @@
         <v>16</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="G23" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>32</v>
@@ -2514,8 +2514,8 @@
       <c r="E24" s="1">
         <v>16</v>
       </c>
-      <c r="F24" s="4">
-        <v>6</v>
+      <c r="F24" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="G24" s="1">
         <v>400</v>

</xml_diff>

<commit_message>
Termino dimensiones y condiciones de apoyo de losas+numeración ult.pisos
</commit_message>
<xml_diff>
--- a/Tarea 05/dimensiones losas.xlsx
+++ b/Tarea 05/dimensiones losas.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive (ignacio.yanez.g@ug.uchile.cl)\Universidad\Semestre 12 Primavera 2018\proyecto de hormigon\proyecto-CI5206\Tarea 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57F8817-36FD-4BBA-9214-8A3CB3181D59}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152EA3F2-FB0E-433B-B8BF-104B7234F973}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{77A8B211-3B65-4AFE-BDB5-07A2739F3869}"/>
   </bookViews>
   <sheets>
     <sheet name="Piso -1" sheetId="1" r:id="rId1"/>
     <sheet name="Piso 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Piso 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Piso 2-7" sheetId="3" r:id="rId3"/>
+    <sheet name="Piso 8-13" sheetId="4" r:id="rId4"/>
+    <sheet name="Piso 14-22" sheetId="5" r:id="rId5"/>
+    <sheet name="Piso 23" sheetId="6" r:id="rId6"/>
+    <sheet name="Piso 24" sheetId="7" r:id="rId7"/>
+    <sheet name="Cubierta" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="155">
   <si>
     <t>N° Losa</t>
   </si>
@@ -103,9 +108,6 @@
     <t>Caso</t>
   </si>
   <si>
-    <t>SC</t>
-  </si>
-  <si>
     <t>Tipo H.</t>
   </si>
   <si>
@@ -133,9 +135,6 @@
     <t>G35</t>
   </si>
   <si>
-    <t>G36</t>
-  </si>
-  <si>
     <t>Lx (m)</t>
   </si>
   <si>
@@ -281,14 +280,244 @@
   </si>
   <si>
     <t>222</t>
+  </si>
+  <si>
+    <t>801</t>
+  </si>
+  <si>
+    <t>802</t>
+  </si>
+  <si>
+    <t>803</t>
+  </si>
+  <si>
+    <t>804</t>
+  </si>
+  <si>
+    <t>805</t>
+  </si>
+  <si>
+    <t>806</t>
+  </si>
+  <si>
+    <t>807</t>
+  </si>
+  <si>
+    <t>808</t>
+  </si>
+  <si>
+    <t>809</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>811</t>
+  </si>
+  <si>
+    <t>812</t>
+  </si>
+  <si>
+    <t>813</t>
+  </si>
+  <si>
+    <t>814</t>
+  </si>
+  <si>
+    <t>815</t>
+  </si>
+  <si>
+    <t>816</t>
+  </si>
+  <si>
+    <t>817</t>
+  </si>
+  <si>
+    <t>818</t>
+  </si>
+  <si>
+    <t>819</t>
+  </si>
+  <si>
+    <t>820</t>
+  </si>
+  <si>
+    <t>821</t>
+  </si>
+  <si>
+    <t>822</t>
+  </si>
+  <si>
+    <t>G30</t>
+  </si>
+  <si>
+    <t>1401</t>
+  </si>
+  <si>
+    <t>1402</t>
+  </si>
+  <si>
+    <t>1403</t>
+  </si>
+  <si>
+    <t>1404</t>
+  </si>
+  <si>
+    <t>1405</t>
+  </si>
+  <si>
+    <t>1406</t>
+  </si>
+  <si>
+    <t>1407</t>
+  </si>
+  <si>
+    <t>1408</t>
+  </si>
+  <si>
+    <t>1409</t>
+  </si>
+  <si>
+    <t>1410</t>
+  </si>
+  <si>
+    <t>1411</t>
+  </si>
+  <si>
+    <t>1412</t>
+  </si>
+  <si>
+    <t>1413</t>
+  </si>
+  <si>
+    <t>1414</t>
+  </si>
+  <si>
+    <t>1415</t>
+  </si>
+  <si>
+    <t>1416</t>
+  </si>
+  <si>
+    <t>1417</t>
+  </si>
+  <si>
+    <t>1418</t>
+  </si>
+  <si>
+    <t>1419</t>
+  </si>
+  <si>
+    <t>1420</t>
+  </si>
+  <si>
+    <t>1421</t>
+  </si>
+  <si>
+    <t>1422</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>2301</t>
+  </si>
+  <si>
+    <t>2302</t>
+  </si>
+  <si>
+    <t>2303</t>
+  </si>
+  <si>
+    <t>2304</t>
+  </si>
+  <si>
+    <t>2305</t>
+  </si>
+  <si>
+    <t>2306</t>
+  </si>
+  <si>
+    <t>2307</t>
+  </si>
+  <si>
+    <t>2308</t>
+  </si>
+  <si>
+    <t>2309</t>
+  </si>
+  <si>
+    <t>2310</t>
+  </si>
+  <si>
+    <t>2311</t>
+  </si>
+  <si>
+    <t>2312</t>
+  </si>
+  <si>
+    <t>2313</t>
+  </si>
+  <si>
+    <t>2314</t>
+  </si>
+  <si>
+    <t>2315</t>
+  </si>
+  <si>
+    <t>2316</t>
+  </si>
+  <si>
+    <t>2317</t>
+  </si>
+  <si>
+    <t>2318</t>
+  </si>
+  <si>
+    <t>2319</t>
+  </si>
+  <si>
+    <t>2320</t>
+  </si>
+  <si>
+    <t>2321</t>
+  </si>
+  <si>
+    <t>2322</t>
+  </si>
+  <si>
+    <t>2401</t>
+  </si>
+  <si>
+    <t>2402</t>
+  </si>
+  <si>
+    <t>2403</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>f'c (tonf/m2)</t>
+  </si>
+  <si>
+    <t>SC (kgf/m2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -310,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -318,11 +547,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -334,6 +583,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -357,16 +633,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>160021</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>137161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>484693</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>137161</xdr:rowOff>
+      <xdr:rowOff>121921</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -699,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7796671-BE69-4D9A-8979-89DC1EB38DCD}">
-  <dimension ref="B3:H32"/>
+  <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,30 +986,43 @@
     <col min="1" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -753,10 +1042,13 @@
         <v>500</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -776,10 +1068,13 @@
         <v>500</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -799,10 +1094,13 @@
         <v>500</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -822,10 +1120,13 @@
         <v>500</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -845,10 +1146,13 @@
         <v>500</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -868,10 +1172,13 @@
         <v>500</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -891,10 +1198,13 @@
         <v>500</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -914,10 +1224,13 @@
         <v>500</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -937,10 +1250,13 @@
         <v>500</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
@@ -960,10 +1276,13 @@
         <v>500</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -983,10 +1302,13 @@
         <v>500</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1006,10 +1328,13 @@
         <v>400</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1029,10 +1354,13 @@
         <v>400</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1052,10 +1380,13 @@
         <v>500</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1075,10 +1406,13 @@
         <v>500</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1098,10 +1432,13 @@
         <v>500</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1121,10 +1458,13 @@
         <v>500</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1144,10 +1484,13 @@
         <v>400</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1167,10 +1510,13 @@
         <v>400</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I22" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1184,16 +1530,19 @@
         <v>17</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G23" s="1">
         <v>400</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1213,12 +1562,15 @@
         <v>400</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1">
         <v>4.25</v>
@@ -1236,12 +1588,15 @@
         <v>500</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
         <v>6.49</v>
@@ -1259,12 +1614,15 @@
         <v>500</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I26" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1">
         <v>8.24</v>
@@ -1282,12 +1640,15 @@
         <v>500</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I27" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1">
         <v>5</v>
@@ -1305,12 +1666,15 @@
         <v>500</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1">
         <v>5.52</v>
@@ -1328,12 +1692,15 @@
         <v>500</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I29" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="1">
         <v>7.09</v>
@@ -1351,12 +1718,15 @@
         <v>500</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>3.6</v>
@@ -1374,74 +1744,85 @@
         <v>500</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="1">
+        <v>31</v>
+      </c>
+      <c r="I31" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="5">
         <v>2.3199999999999998</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="5">
         <v>4.3</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="5">
         <v>17</v>
       </c>
-      <c r="F32" s="1">
-        <v>6</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="F32" s="5">
+        <v>6</v>
+      </c>
+      <c r="G32" s="5">
         <v>400</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>33</v>
+      <c r="H32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="5">
+        <v>3.57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB8B69-A653-4E8B-A8D1-A28FAE860C51}">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -1453,18 +1834,21 @@
         <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1">
         <v>500</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
@@ -1482,12 +1866,15 @@
         <v>500</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>
@@ -1505,12 +1892,15 @@
         <v>500</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -1528,12 +1918,15 @@
         <v>500</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>4.93</v>
@@ -1551,12 +1944,15 @@
         <v>500</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1">
         <v>5.54</v>
@@ -1574,12 +1970,15 @@
         <v>500</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1">
         <v>5.54</v>
@@ -1597,12 +1996,15 @@
         <v>500</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1">
         <v>5.54</v>
@@ -1620,12 +2022,15 @@
         <v>500</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1">
         <v>5.54</v>
@@ -1637,18 +2042,21 @@
         <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1">
         <v>500</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1">
         <v>4.6500000000000004</v>
@@ -1666,12 +2074,15 @@
         <v>400</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1">
         <v>4.6500000000000004</v>
@@ -1689,12 +2100,15 @@
         <v>500</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1">
         <v>6.05</v>
@@ -1712,12 +2126,15 @@
         <v>500</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1735,12 +2152,15 @@
         <v>400</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1">
         <v>1.4</v>
@@ -1758,12 +2178,15 @@
         <v>400</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1">
         <v>2.9</v>
@@ -1781,12 +2204,15 @@
         <v>400</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1804,12 +2230,15 @@
         <v>200</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1">
         <v>5.82</v>
@@ -1827,12 +2256,15 @@
         <v>200</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1">
         <v>1.34</v>
@@ -1844,18 +2276,21 @@
         <v>16</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G20" s="1">
         <v>300</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1">
         <v>2.1</v>
@@ -1867,39 +2302,45 @@
         <v>16</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" s="1">
         <v>400</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="1">
+        <v>31</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="5">
         <v>2.3199999999999998</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="5">
         <v>4.3</v>
       </c>
-      <c r="E22" s="1">
-        <v>16</v>
-      </c>
-      <c r="F22" s="4">
-        <v>6</v>
-      </c>
-      <c r="G22" s="1">
+      <c r="E22" s="5">
+        <v>16</v>
+      </c>
+      <c r="F22" s="8">
+        <v>6</v>
+      </c>
+      <c r="G22" s="5">
         <v>400</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="5">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1907,8 +2348,9 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1916,8 +2358,9 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1926,7 +2369,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1935,7 +2378,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1944,7 +2387,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1953,7 +2396,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1962,7 +2405,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1971,7 +2414,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1987,40 +2430,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CFD12D-4AE1-4F93-8131-51CD10C27189}">
-  <dimension ref="B2:H24"/>
+  <dimension ref="B1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B24" sqref="B24:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1">
         <v>6.05</v>
@@ -2038,12 +2485,15 @@
         <v>200</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1">
         <v>4.6500000000000004</v>
@@ -2061,12 +2511,15 @@
         <v>200</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <v>4.6500000000000004</v>
@@ -2084,12 +2537,15 @@
         <v>200</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1">
         <v>6.05</v>
@@ -2107,12 +2563,15 @@
         <v>200</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1">
         <v>5.82</v>
@@ -2130,12 +2589,15 @@
         <v>200</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
@@ -2153,12 +2615,15 @@
         <v>200</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="1">
         <v>2.1</v>
@@ -2170,18 +2635,21 @@
         <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>400</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1">
         <v>1.4</v>
@@ -2199,12 +2667,15 @@
         <v>400</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1">
         <v>2.9</v>
@@ -2222,12 +2693,15 @@
         <v>400</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
@@ -2245,12 +2719,15 @@
         <v>200</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1">
         <v>5.82</v>
@@ -2268,12 +2745,15 @@
         <v>200</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1">
         <v>1.51</v>
@@ -2285,18 +2765,21 @@
         <v>16</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G14" s="1">
         <v>300</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="1">
         <v>1.51</v>
@@ -2308,18 +2791,21 @@
         <v>16</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G15" s="1">
         <v>300</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1">
         <v>1.51</v>
@@ -2331,18 +2817,21 @@
         <v>16</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G16" s="1">
         <v>300</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1">
         <v>1.51</v>
@@ -2354,18 +2843,21 @@
         <v>16</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G17" s="1">
         <v>300</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C18" s="1">
         <v>1.04</v>
@@ -2377,18 +2869,21 @@
         <v>16</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
         <v>300</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1">
         <v>1.04</v>
@@ -2400,18 +2895,21 @@
         <v>16</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G19" s="1">
         <v>300</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1">
         <v>1.34</v>
@@ -2423,18 +2921,21 @@
         <v>16</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G20" s="1">
         <v>300</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="1">
         <v>1.34</v>
@@ -2446,18 +2947,21 @@
         <v>16</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G21" s="1">
         <v>300</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C22" s="1">
         <v>0.74</v>
@@ -2469,18 +2973,21 @@
         <v>16</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G22" s="1">
         <v>300</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I22" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1">
         <v>0.7</v>
@@ -2492,37 +2999,2136 @@
         <v>16</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G23" s="1">
         <v>300</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>16</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="5">
+        <v>400</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="5">
+        <v>3.57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF85145-DA80-4684-9F71-43CEC63D9AC2}">
+  <dimension ref="B1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1">
+        <v>200</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C4" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>200</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>200</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>200</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.96</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
+        <v>200</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.04</v>
+      </c>
+      <c r="E9" s="1">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1">
+        <v>400</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>400</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6.36</v>
+      </c>
+      <c r="E11" s="1">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>400</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>200</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>200</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.33</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="1">
+        <v>300</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="1">
+        <v>300</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="1">
+        <v>300</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="1">
+        <v>300</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="1">
+        <v>300</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="1">
+        <v>300</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7.01</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="1">
+        <v>300</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7.09</v>
+      </c>
+      <c r="E21" s="1">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1">
+        <v>300</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="1">
+        <v>300</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E23" s="1">
+        <v>16</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="1">
+        <v>300</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="5">
         <v>2.3199999999999998</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="5">
         <v>4.3</v>
       </c>
-      <c r="E24" s="1">
-        <v>16</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="E24" s="5">
+        <v>16</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="5">
         <v>400</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" s="5">
+        <v>3.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847EB0DE-B014-4C2B-AD6C-26B0E85CF6CB}">
+  <dimension ref="B1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1">
+        <v>200</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>200</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>200</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>200</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.96</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
+        <v>200</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.04</v>
+      </c>
+      <c r="E9" s="1">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1">
+        <v>400</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>400</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6.36</v>
+      </c>
+      <c r="E11" s="1">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>400</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>200</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>200</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.33</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="1">
+        <v>300</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="1">
+        <v>300</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="1">
+        <v>300</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="1">
+        <v>300</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="1">
+        <v>300</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="1">
+        <v>300</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7.01</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="1">
+        <v>300</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7.09</v>
+      </c>
+      <c r="E21" s="1">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1">
+        <v>300</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="1">
+        <v>300</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="D23" s="12">
+        <v>3.83</v>
+      </c>
+      <c r="E23" s="12">
+        <v>16</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="12">
+        <v>300</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="12">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>16</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="5">
+        <v>400</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="5">
+        <v>2.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA95C36-310C-43EE-A872-618577F28BEF}">
+  <dimension ref="B1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B23:I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>100</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.96</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>100</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E8" s="1">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
+        <v>100</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.04</v>
+      </c>
+      <c r="E9" s="1">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>100</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6.36</v>
+      </c>
+      <c r="E11" s="1">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>100</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>100</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>100</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.51</v>
+      </c>
+      <c r="D14" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="1">
+        <v>100</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="1">
+        <v>100</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="1">
+        <v>100</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.51</v>
+      </c>
+      <c r="D17" s="3">
+        <v>8.93</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="1">
+        <v>100</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16</v>
+      </c>
+      <c r="F18" s="3">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <v>100</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
+        <v>100</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.34</v>
+      </c>
+      <c r="D20" s="3">
+        <v>10.69</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="1">
+        <v>100</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1.34</v>
+      </c>
+      <c r="D21" s="3">
+        <v>10.86</v>
+      </c>
+      <c r="E21" s="1">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1">
+        <v>100</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4</v>
+      </c>
+      <c r="G22" s="1">
+        <v>100</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="D23" s="12">
+        <v>3.83</v>
+      </c>
+      <c r="E23" s="12">
+        <v>16</v>
+      </c>
+      <c r="F23" s="13">
+        <v>4</v>
+      </c>
+      <c r="G23" s="12">
+        <v>100</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="12">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>16</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="5">
+        <v>100</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="5">
+        <v>2.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3AB66-6A5F-4CAF-B31E-18AD20C84E2D}">
+  <dimension ref="B1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.04</v>
+      </c>
+      <c r="E3" s="1">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.9</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6.36</v>
+      </c>
+      <c r="E5" s="5">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5">
+        <v>100</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6450CBA-39C9-46BB-83D0-7BC62DBE551F}">
+  <dimension ref="B2:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4" s="10">
+        <v>4.04</v>
+      </c>
+      <c r="E4" s="10">
+        <v>16</v>
+      </c>
+      <c r="F4" s="10">
+        <v>6</v>
+      </c>
+      <c r="G4" s="10">
+        <v>100</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="10">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
añado losa 121 en piso 1
</commit_message>
<xml_diff>
--- a/Tarea 05/dimensiones losas.xlsx
+++ b/Tarea 05/dimensiones losas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive (ignacio.yanez.g@ug.uchile.cl)\Universidad\Semestre 12 Primavera 2018\proyecto de hormigon\proyecto-CI5206\Tarea 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152EA3F2-FB0E-433B-B8BF-104B7234F973}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938ECCF9-836A-4953-8685-57172AA8437B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{77A8B211-3B65-4AFE-BDB5-07A2739F3869}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{77A8B211-3B65-4AFE-BDB5-07A2739F3869}"/>
   </bookViews>
   <sheets>
     <sheet name="Piso -1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="156">
   <si>
     <t>N° Losa</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>SC (kgf/m2)</t>
+  </si>
+  <si>
+    <t>121</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -612,11 +615,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -633,16 +654,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>160021</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449581</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>137161</xdr:rowOff>
+      <xdr:rowOff>182881</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>484693</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>774253</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>121921</xdr:rowOff>
+      <xdr:rowOff>167641</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -665,7 +686,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6499861" y="320041"/>
+          <a:off x="8374381" y="365761"/>
           <a:ext cx="2702112" cy="2194560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -977,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7796671-BE69-4D9A-8979-89DC1EB38DCD}">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1785,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB8B69-A653-4E8B-A8D1-A28FAE860C51}">
-  <dimension ref="B1:I31"/>
+  <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2314,41 +2335,57 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="12">
         <v>2.3199999999999998</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="12">
         <v>4.3</v>
       </c>
-      <c r="E22" s="5">
-        <v>16</v>
-      </c>
-      <c r="F22" s="8">
-        <v>6</v>
-      </c>
-      <c r="G22" s="5">
+      <c r="E22" s="12">
+        <v>16</v>
+      </c>
+      <c r="F22" s="14">
+        <v>6</v>
+      </c>
+      <c r="G22" s="12">
         <v>400</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="H22" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="12">
         <v>3.57</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="B23" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="D23" s="12">
+        <v>6.05</v>
+      </c>
+      <c r="E23" s="12">
+        <v>16</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="12">
+        <v>400</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="12">
+        <v>3.57</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
@@ -2368,6 +2405,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
@@ -2422,6 +2460,15 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="2"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2433,7 +2480,7 @@
   <dimension ref="B1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:I24"/>
+      <selection activeCell="J3" sqref="J3:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>